<commit_message>
Update code that produces fiure 5 of manuscript to meet minor revision.
</commit_message>
<xml_diff>
--- a/Running_and_analysing_simulations/parameters/Parameters values in LHS Sports Match Sims.xlsx
+++ b/Running_and_analysing_simulations/parameters/Parameters values in LHS Sports Match Sims.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdgru\OneDrive\Documents\GitHub\Modelling-Disease-Mitigation-at-Mass-Gatherings-A-Case-Study-of-COVID-19-at-the-2022-FIFA-World-Cup\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdgru\OneDrive\Documents\GitHub\Modelling-Disease-Mitigation-at-Mass-Gatherings-A-Case-Study-of-COVID-19-at-the-2022-FIFA-World-Cup\Running_and_analysing_simulations\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD5C332-B9FB-44CE-AA16-27B635F905A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FF8DA8-BC52-4613-88B7-66A42278B53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="99">
   <si>
     <t>Parameter</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t>tau_{RA} low</t>
-  </si>
-  <si>
-    <t>tau_{RA} high</t>
   </si>
 </sst>
 </file>
@@ -624,10 +621,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F990"/>
+  <dimension ref="A1:F989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1117,144 +1114,133 @@
     </row>
     <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="1">
-        <v>0.81299999999999994</v>
+      <c r="E30" s="3">
+        <v>0.96799999999999997</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>2930524</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3">
-        <v>2930524</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C34" s="3">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="D34" s="3">
-        <v>0.5</v>
+        <v>20000</v>
       </c>
       <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="3">
-        <v>4000</v>
-      </c>
-      <c r="D35" s="3">
-        <v>20000</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="7">
+        <v>2848639</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="7">
-        <v>2848639</v>
+        <v>1898869</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="7">
-        <v>1898869</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4000</v>
+      </c>
+      <c r="D37" s="3">
+        <v>80000</v>
+      </c>
+      <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="3">
-        <v>4000</v>
-      </c>
-      <c r="D38" s="3">
-        <v>80000</v>
-      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -6011,11 +5997,6 @@
       <c r="C989" s="3"/>
       <c r="D989" s="3"/>
       <c r="E989" s="3"/>
-    </row>
-    <row r="990" spans="3:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C990" s="3"/>
-      <c r="D990" s="3"/>
-      <c r="E990" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>